<commit_message>
Moved previous day check to own loop. Added bool for working days.
</commit_message>
<xml_diff>
--- a/Data/Corrected.xlsx
+++ b/Data/Corrected.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10106"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Cameron/Library/Mobile Documents/com~apple~CloudDocs/iCloud Storage/Other/RonAccounting/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carolinejudge/Library/Mobile Documents/com~apple~CloudDocs/Desktop/Cameron/RonAccounting/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12ECC106-09A5-6E4A-A1E1-BC1D08CF3CA1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54749203-CCD1-1347-AF6F-6C892640C3C9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="16300" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Payroll FOH" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Payroll FOH'!$A$1:$K$123</definedName>
   </definedNames>
-  <calcPr calcId="191028" concurrentCalc="0"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -917,7 +917,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -967,6 +967,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -1313,27 +1314,27 @@
   <dimension ref="A1:Y123"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="W2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="M2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1"/>
-      <selection pane="bottomRight" activeCell="X4" sqref="X4"/>
+      <selection pane="bottomRight" activeCell="Y3" sqref="Y3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8515625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="32.80078125" customWidth="1"/>
-    <col min="2" max="2" width="21.20703125" customWidth="1"/>
-    <col min="3" max="3" width="11.9609375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="11.46484375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="25.27734375" customWidth="1"/>
-    <col min="6" max="6" width="23.55078125" customWidth="1"/>
-    <col min="7" max="7" width="10.8515625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="14.0546875" style="3" customWidth="1"/>
-    <col min="9" max="9" width="14.55078125" style="3" customWidth="1"/>
-    <col min="10" max="10" width="10.97265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.8515625" style="2"/>
-    <col min="12" max="13" width="10.8515625" style="3"/>
-    <col min="15" max="15" width="24.78515625" customWidth="1"/>
+    <col min="1" max="1" width="32.83203125" customWidth="1"/>
+    <col min="2" max="2" width="21.1640625" customWidth="1"/>
+    <col min="3" max="3" width="12" style="2" customWidth="1"/>
+    <col min="4" max="4" width="11.5" style="2" customWidth="1"/>
+    <col min="5" max="5" width="25.33203125" customWidth="1"/>
+    <col min="6" max="6" width="23.5" customWidth="1"/>
+    <col min="7" max="7" width="10.83203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="14" style="3" customWidth="1"/>
+    <col min="9" max="9" width="14.5" style="3" customWidth="1"/>
+    <col min="10" max="10" width="11" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.83203125" style="2"/>
+    <col min="12" max="13" width="10.83203125" style="3"/>
+    <col min="15" max="15" width="24.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.2">
@@ -1407,7 +1408,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:25" ht="15" x14ac:dyDescent="0.2">
       <c r="O2" t="s">
         <v>229</v>
       </c>
@@ -1448,7 +1449,7 @@
         <v>670.55372106666664</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:25" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>72</v>
       </c>
@@ -1486,44 +1487,44 @@
       <c r="O3" t="s">
         <v>230</v>
       </c>
-      <c r="P3" s="14">
+      <c r="P3" s="27">
         <f>SUMIF($A$26:$A$120,"=Tatiana B.",$G$26:$G$120)/2</f>
         <v>37.316110900000005</v>
       </c>
-      <c r="Q3" s="14">
+      <c r="Q3" s="27">
         <f>SUMIF($A$26:$A$120,"=JESSICA B.",$G$26:$G$120)/2</f>
         <v>15.368055500000001</v>
       </c>
-      <c r="R3" s="14">
+      <c r="R3" s="27">
         <f>SUMIF($A$26:$A$120,"=Elijah Szelag",$G$26:$G$120)/2</f>
         <v>35.057499799999995</v>
       </c>
-      <c r="S3" s="14">
+      <c r="S3" s="27">
         <f>SUMIF($A$26:$A$120,"=Daniel P.",$G$26:$G$120)/2</f>
         <v>0</v>
       </c>
-      <c r="T3" s="14">
+      <c r="T3" s="27">
         <f>SUMIF($A$26:$A$120,"=Jarren",$G$26:$G$120)/2</f>
         <v>19.079444300000002</v>
       </c>
-      <c r="U3" s="14">
+      <c r="U3" s="27">
         <f>SUMIF($A$26:$A$120,"=Jessa R",$G$26:$G$120)/2</f>
         <v>18.262777700000001</v>
       </c>
-      <c r="V3" s="14">
+      <c r="V3" s="27">
         <f>SUMIF($A$26:$A$120,"=Katie D",$G$26:$G$120)/2</f>
         <v>14.7563888</v>
       </c>
-      <c r="W3" s="14">
+      <c r="W3" s="27">
         <f>SUMIF($A$26:$A$120,"=Trina",$G$26:$G$120)/2</f>
         <v>20.746388799999998</v>
       </c>
-      <c r="X3" s="14">
+      <c r="X3" s="27">
         <f>SUMIF($A$26:$A$120,"=Tori M",$G$26:$G$120)/2</f>
         <v>32.244444299999998</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:25" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>72</v>
       </c>
@@ -1598,7 +1599,7 @@
         <v>257.95555439999998</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:25" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>106</v>
       </c>
@@ -1673,7 +1674,7 @@
         <v>412.59816666666671</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:25" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>106</v>
       </c>
@@ -1745,7 +1746,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:25" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>116</v>
       </c>
@@ -1781,7 +1782,7 @@
         <v>close</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:25" ht="15" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>116</v>
       </c>
@@ -1831,7 +1832,7 @@
       <c r="W8" s="22"/>
       <c r="X8" s="22"/>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:25" ht="15" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>129</v>
       </c>
@@ -1882,7 +1883,7 @@
       <c r="W9" s="22"/>
       <c r="X9" s="22"/>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:25" ht="15" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>129</v>
       </c>
@@ -1930,7 +1931,7 @@
       <c r="W10" s="22"/>
       <c r="X10" s="22"/>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:25" ht="15" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>138</v>
       </c>
@@ -2002,7 +2003,7 @@
         <v>257.95555439999998</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:25" ht="15" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>138</v>
       </c>
@@ -2050,7 +2051,7 @@
       <c r="W12" s="22"/>
       <c r="X12" s="22"/>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:25" ht="15" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>173</v>
       </c>
@@ -2101,7 +2102,7 @@
       <c r="W13" s="22"/>
       <c r="X13" s="22"/>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:25" ht="15" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>173</v>
       </c>
@@ -2152,7 +2153,7 @@
       <c r="W14" s="22"/>
       <c r="X14" s="22"/>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:25" ht="15" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>173</v>
       </c>
@@ -2202,7 +2203,7 @@
       <c r="W15" s="22"/>
       <c r="X15" s="22"/>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:25" ht="15" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>190</v>
       </c>
@@ -2238,7 +2239,7 @@
         <v>close</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:15" ht="15" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>190</v>
       </c>
@@ -2274,7 +2275,7 @@
         <v>close</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:15" ht="15" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>190</v>
       </c>
@@ -2310,7 +2311,7 @@
         <v>close</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:15" ht="15" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>190</v>
       </c>
@@ -2349,7 +2350,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:15" ht="15" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>204</v>
       </c>
@@ -2388,7 +2389,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:15" ht="15" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>204</v>
       </c>
@@ -2427,7 +2428,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:15" ht="15" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>204</v>
       </c>
@@ -2466,12 +2467,12 @@
         <v>251</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:15" ht="15" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:15" ht="15" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>116</v>
       </c>
@@ -2515,7 +2516,7 @@
         <v>82.022221599999995</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:15" ht="15" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>116</v>
       </c>
@@ -2551,7 +2552,7 @@
         <v>close</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:15" ht="15" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>190</v>
       </c>
@@ -2596,7 +2597,7 @@
         <v>76.791110400000008</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:15" ht="15" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>190</v>
       </c>
@@ -2633,7 +2634,7 @@
         <v>close</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:15" ht="15" x14ac:dyDescent="0.2">
       <c r="A30" s="8" t="s">
         <v>239</v>
       </c>
@@ -2646,7 +2647,7 @@
         <v>35.5</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:15" ht="15" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>72</v>
       </c>
@@ -2687,7 +2688,7 @@
         <v>172.51555519999999</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>72</v>
       </c>
@@ -2720,7 +2721,7 @@
         <v>open</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A34" s="8" t="s">
         <v>239</v>
       </c>
@@ -2733,12 +2734,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>173</v>
       </c>
@@ -2782,7 +2783,7 @@
         <v>113.6777776</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>173</v>
       </c>
@@ -2818,7 +2819,7 @@
         <v>close</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>204</v>
       </c>
@@ -2862,7 +2863,7 @@
         <v>111.9155552</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>204</v>
       </c>
@@ -2898,7 +2899,7 @@
         <v>close</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A42" s="8" t="s">
         <v>239</v>
       </c>
@@ -2911,7 +2912,7 @@
         <v>60.3</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>72</v>
       </c>
@@ -2955,7 +2956,7 @@
         <v>217.824444</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>72</v>
       </c>
@@ -2991,7 +2992,7 @@
         <v>open</v>
       </c>
     </row>
-    <row r="46" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:13" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="8" t="s">
         <v>239</v>
       </c>
@@ -3004,7 +3005,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>242</v>
       </c>
@@ -3429,7 +3430,7 @@
         <v>open</v>
       </c>
     </row>
-    <row r="62" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:13" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="8" t="s">
         <v>239</v>
       </c>
@@ -4174,7 +4175,7 @@
         <v>open</v>
       </c>
     </row>
-    <row r="86" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:13" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="8" t="s">
         <v>239</v>
       </c>
@@ -4884,7 +4885,7 @@
       </c>
       <c r="L108" s="13"/>
     </row>
-    <row r="109" spans="1:15" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:15" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" s="8" t="s">
         <v>239</v>
       </c>
@@ -5291,25 +5292,25 @@
   <dimension ref="A1:K68"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B17" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomRight" activeCell="B71" sqref="B71"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8515625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="32.80078125" customWidth="1"/>
-    <col min="2" max="2" width="20.09765625" customWidth="1"/>
-    <col min="3" max="3" width="11.9609375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="11.46484375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="25.27734375" customWidth="1"/>
-    <col min="6" max="6" width="23.55078125" customWidth="1"/>
-    <col min="7" max="7" width="10.8515625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="14.0546875" style="3" customWidth="1"/>
-    <col min="9" max="9" width="14.55078125" style="3" customWidth="1"/>
-    <col min="10" max="10" width="10.97265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.8515625" style="2"/>
+    <col min="1" max="1" width="32.83203125" customWidth="1"/>
+    <col min="2" max="2" width="20.1640625" customWidth="1"/>
+    <col min="3" max="3" width="12" style="2" customWidth="1"/>
+    <col min="4" max="4" width="11.5" style="2" customWidth="1"/>
+    <col min="5" max="5" width="25.33203125" customWidth="1"/>
+    <col min="6" max="6" width="23.5" customWidth="1"/>
+    <col min="7" max="7" width="10.83203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="14" style="3" customWidth="1"/>
+    <col min="9" max="9" width="14.5" style="3" customWidth="1"/>
+    <col min="10" max="10" width="11" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.2">
@@ -5347,7 +5348,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
         <v>20</v>
       </c>
@@ -5383,7 +5384,7 @@
         <v>close</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -5419,7 +5420,7 @@
         <v>close</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -5455,7 +5456,7 @@
         <v>open</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -5491,7 +5492,7 @@
         <v>open</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -5527,7 +5528,7 @@
         <v>close</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -5563,7 +5564,7 @@
         <v>close</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -5599,7 +5600,7 @@
         <v>open</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -5635,7 +5636,7 @@
         <v>open</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -5671,7 +5672,7 @@
         <v>open</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -5707,7 +5708,7 @@
         <v>open</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A12" s="19" t="s">
         <v>36</v>
       </c>
@@ -5743,7 +5744,7 @@
         <v>close</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>36</v>
       </c>
@@ -5779,7 +5780,7 @@
         <v>close</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>36</v>
       </c>
@@ -5815,7 +5816,7 @@
         <v>open</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>36</v>
       </c>
@@ -5851,7 +5852,7 @@
         <v>open</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>36</v>
       </c>
@@ -5887,7 +5888,7 @@
         <v>open</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>36</v>
       </c>
@@ -5923,7 +5924,7 @@
         <v>open</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>36</v>
       </c>
@@ -5959,7 +5960,7 @@
         <v>open</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>36</v>
       </c>
@@ -5995,7 +5996,7 @@
         <v>open</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>36</v>
       </c>
@@ -6031,7 +6032,7 @@
         <v>close</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>36</v>
       </c>
@@ -6067,7 +6068,7 @@
         <v>close</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>36</v>
       </c>
@@ -6103,7 +6104,7 @@
         <v>open</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>36</v>
       </c>
@@ -6139,7 +6140,7 @@
         <v>open</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>36</v>
       </c>
@@ -6175,7 +6176,7 @@
         <v>open</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>36</v>
       </c>
@@ -6211,7 +6212,7 @@
         <v>open</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>36</v>
       </c>
@@ -6247,7 +6248,7 @@
         <v>open</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A27" s="19" t="s">
         <v>57</v>
       </c>
@@ -6283,7 +6284,7 @@
         <v>close</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>57</v>
       </c>
@@ -6319,7 +6320,7 @@
         <v>close</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>57</v>
       </c>
@@ -6355,7 +6356,7 @@
         <v>open</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>57</v>
       </c>
@@ -6391,7 +6392,7 @@
         <v>open</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>57</v>
       </c>
@@ -6427,7 +6428,7 @@
         <v>open</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>57</v>
       </c>
@@ -6463,7 +6464,7 @@
         <v>open</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>57</v>
       </c>
@@ -6499,7 +6500,7 @@
         <v>close</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>57</v>
       </c>
@@ -6535,7 +6536,7 @@
         <v>close</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>57</v>
       </c>
@@ -6571,7 +6572,7 @@
         <v>close</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>57</v>
       </c>
@@ -6607,7 +6608,7 @@
         <v>close</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>57</v>
       </c>
@@ -6643,7 +6644,7 @@
         <v>open</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>57</v>
       </c>
@@ -6679,7 +6680,7 @@
         <v>open</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>86</v>
       </c>
@@ -6715,7 +6716,7 @@
         <v>close</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>86</v>
       </c>
@@ -6751,7 +6752,7 @@
         <v>close</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>86</v>
       </c>
@@ -6787,7 +6788,7 @@
         <v>open</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>86</v>
       </c>
@@ -6823,7 +6824,7 @@
         <v>open</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A43" s="19" t="s">
         <v>89</v>
       </c>
@@ -6859,7 +6860,7 @@
         <v>close</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>89</v>
       </c>
@@ -6895,7 +6896,7 @@
         <v>close</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>89</v>
       </c>
@@ -6931,7 +6932,7 @@
         <v>open</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>89</v>
       </c>
@@ -6967,7 +6968,7 @@
         <v>open</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>89</v>
       </c>
@@ -7003,7 +7004,7 @@
         <v>close</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>89</v>
       </c>
@@ -7039,7 +7040,7 @@
         <v>close</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>89</v>
       </c>
@@ -7075,7 +7076,7 @@
         <v>close</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>89</v>
       </c>
@@ -7111,7 +7112,7 @@
         <v>close</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>89</v>
       </c>
@@ -7147,7 +7148,7 @@
         <v>close</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>89</v>
       </c>
@@ -7183,7 +7184,7 @@
         <v>close</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>89</v>
       </c>
@@ -7219,7 +7220,7 @@
         <v>open</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>89</v>
       </c>
@@ -7255,7 +7256,7 @@
         <v>open</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>89</v>
       </c>
@@ -7291,7 +7292,7 @@
         <v>close</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A56" s="19" t="s">
         <v>159</v>
       </c>
@@ -7327,7 +7328,7 @@
         <v>close</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>159</v>
       </c>
@@ -7363,7 +7364,7 @@
         <v>close</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>159</v>
       </c>
@@ -7399,7 +7400,7 @@
         <v>close</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>159</v>
       </c>
@@ -7435,7 +7436,7 @@
         <v>close</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>159</v>
       </c>
@@ -7471,7 +7472,7 @@
         <v>close</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>159</v>
       </c>
@@ -7507,7 +7508,7 @@
         <v>close</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>159</v>
       </c>
@@ -7543,7 +7544,7 @@
         <v>close</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>159</v>
       </c>
@@ -7579,7 +7580,7 @@
         <v>close</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>159</v>
       </c>
@@ -7739,10 +7740,10 @@
   <dimension ref="B3:L20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8515625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="3" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B3" s="19" t="s">

</xml_diff>

<commit_message>
Rounded out tips by shift for doubles. Averages coworkers tips by shift.
</commit_message>
<xml_diff>
--- a/Data/Corrected.xlsx
+++ b/Data/Corrected.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10207"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carolinejudge/Library/Mobile Documents/com~apple~CloudDocs/Desktop/Cameron/RonAccounting/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cameron/Library/Mobile Documents/com~apple~CloudDocs/iCloud Storage/Other/RonAccounting/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54749203-CCD1-1347-AF6F-6C892640C3C9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66C48244-437F-D54A-A493-F7FE7236DA3D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="17080" windowHeight="26600" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Payroll FOH" sheetId="1" r:id="rId1"/>
@@ -1313,24 +1313,23 @@
   </sheetPr>
   <dimension ref="A1:Y123"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="M2" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Y3" sqref="Y3"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="32.83203125" customWidth="1"/>
-    <col min="2" max="2" width="21.1640625" customWidth="1"/>
-    <col min="3" max="3" width="12" style="2" customWidth="1"/>
-    <col min="4" max="4" width="11.5" style="2" customWidth="1"/>
-    <col min="5" max="5" width="25.33203125" customWidth="1"/>
-    <col min="6" max="6" width="23.5" customWidth="1"/>
-    <col min="7" max="7" width="10.83203125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="14" style="3" customWidth="1"/>
-    <col min="9" max="9" width="14.5" style="3" customWidth="1"/>
+    <col min="1" max="1" width="18.33203125" customWidth="1"/>
+    <col min="2" max="2" width="7.5" customWidth="1"/>
+    <col min="3" max="3" width="6.5" style="2" customWidth="1"/>
+    <col min="4" max="4" width="6.83203125" style="2" customWidth="1"/>
+    <col min="5" max="6" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.5" style="3" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11" style="3" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10.83203125" style="2"/>
     <col min="12" max="13" width="10.83203125" style="3"/>
@@ -7076,7 +7075,7 @@
         <v>close</v>
       </c>
     </row>
-    <row r="50" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>89</v>
       </c>
@@ -7112,7 +7111,7 @@
         <v>close</v>
       </c>
     </row>
-    <row r="51" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>89</v>
       </c>
@@ -7148,7 +7147,7 @@
         <v>close</v>
       </c>
     </row>
-    <row r="52" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>89</v>
       </c>
@@ -7184,7 +7183,7 @@
         <v>close</v>
       </c>
     </row>
-    <row r="53" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>89</v>
       </c>
@@ -7220,7 +7219,7 @@
         <v>open</v>
       </c>
     </row>
-    <row r="54" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>89</v>
       </c>
@@ -7256,7 +7255,7 @@
         <v>open</v>
       </c>
     </row>
-    <row r="55" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>89</v>
       </c>
@@ -7292,7 +7291,7 @@
         <v>close</v>
       </c>
     </row>
-    <row r="56" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A56" s="19" t="s">
         <v>159</v>
       </c>
@@ -7328,7 +7327,7 @@
         <v>close</v>
       </c>
     </row>
-    <row r="57" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>159</v>
       </c>
@@ -7364,7 +7363,7 @@
         <v>close</v>
       </c>
     </row>
-    <row r="58" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>159</v>
       </c>
@@ -7400,7 +7399,7 @@
         <v>close</v>
       </c>
     </row>
-    <row r="59" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>159</v>
       </c>
@@ -7436,7 +7435,7 @@
         <v>close</v>
       </c>
     </row>
-    <row r="60" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>159</v>
       </c>
@@ -7472,7 +7471,7 @@
         <v>close</v>
       </c>
     </row>
-    <row r="61" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>159</v>
       </c>
@@ -7508,7 +7507,7 @@
         <v>close</v>
       </c>
     </row>
-    <row r="62" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>159</v>
       </c>
@@ -7544,7 +7543,7 @@
         <v>close</v>
       </c>
     </row>
-    <row r="63" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>159</v>
       </c>
@@ -7580,7 +7579,7 @@
         <v>close</v>
       </c>
     </row>
-    <row r="64" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>159</v>
       </c>
@@ -7739,11 +7738,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FC9748E-E81A-C04D-A33A-010EE0F2B74C}">
   <dimension ref="B3:L20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="6" max="6" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="3" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B3" s="19" t="s">

</xml_diff>